<commit_message>
Data scraped from 2024 season
</commit_message>
<xml_diff>
--- a/Comparing_UNC.xlsx
+++ b/Comparing_UNC.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnb/Personal_Portfolio_Projects/CBB_Score_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnb/Personal_Portfolio_Projects/CBB_Score_Predictor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{306D608B-3DB1-D244-8B61-69C6DA9C16A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46B907C-8C4C-F440-A230-D0EE9DA410CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{3600C094-1DED-FA47-BC99-CC168A066B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>Home</t>
   </si>
@@ -114,6 +114,36 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Home Diff</t>
+  </si>
+  <si>
+    <t>Away Diff</t>
+  </si>
+  <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>Margin Diff</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Clemson</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Florida State</t>
   </si>
 </sst>
 </file>
@@ -151,14 +181,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -211,16 +244,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA3F3503-6195-2B48-A3E7-2699EF9BB823}" name="Table2" displayName="Table2" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17" xr:uid="{DA3F3503-6195-2B48-A3E7-2699EF9BB823}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{42140F0C-9DC2-4E46-9B7A-3FF35D30F9BB}" name="Home" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D6487EF3-73E9-5343-B5E2-45D8F4916148}" name="Away" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA3F3503-6195-2B48-A3E7-2699EF9BB823}" name="Table2" displayName="Table2" ref="A1:F27" totalsRowShown="0">
+  <autoFilter ref="A1:F27" xr:uid="{DA3F3503-6195-2B48-A3E7-2699EF9BB823}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{42140F0C-9DC2-4E46-9B7A-3FF35D30F9BB}" name="Home" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D6487EF3-73E9-5343-B5E2-45D8F4916148}" name="Away" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{6B2B5256-F3CE-4141-BC8D-813A72758740}" name="Home Points"/>
     <tableColumn id="4" xr3:uid="{34B29550-BC0E-5844-BECD-F257B946E23F}" name="Away Points"/>
+    <tableColumn id="7" xr3:uid="{E1CAB575-BB7E-CF47-BE6D-4CD12A02E8AD}" name="Marin" dataDxfId="0">
+      <calculatedColumnFormula>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" xr3:uid="{C1CE8085-BB22-B244-8E8A-F28C8A524CFF}" name="Win / Loss"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A03A250D-ACC0-D54B-8A8C-B9D0AD9FA28B}" name="Table3" displayName="Table3" ref="H1:M27" totalsRowShown="0">
+  <autoFilter ref="H1:M27" xr:uid="{A03A250D-ACC0-D54B-8A8C-B9D0AD9FA28B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D6253092-AAA9-FF46-850E-7F0A560CB6F8}" name="Actual Home"/>
+    <tableColumn id="2" xr3:uid="{0F53744D-5190-E841-B0DA-33ABF3827324}" name="Actual Away"/>
+    <tableColumn id="3" xr3:uid="{76B4E44D-572E-CA45-9806-5C953C833D75}" name="Home Diff">
+      <calculatedColumnFormula>ABS(Table2[[#This Row],[Home Points]]-H2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{95DD1442-108D-8147-932D-7A57058AEADD}" name="Away Diff">
+      <calculatedColumnFormula>ABS(Table2[[#This Row],[Away Points]]-I2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{DF760BC6-123D-C643-B359-3990D5443998}" name="Margin">
+      <calculatedColumnFormula>ABS(H2-I2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B7CB03C1-7392-3F4B-9D12-BED47185A777}" name="Margin Diff">
+      <calculatedColumnFormula>ABS(Table2[[#This Row],[Marin]]-L2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -521,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F4035B-59EE-B34B-A710-8F4302E8ACA3}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,12 +591,15 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,16 +613,31 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -573,17 +650,37 @@
       <c r="D2">
         <v>56</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>86</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H2)</f>
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I2)</f>
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <f>ABS(H2-I2)</f>
+        <v>17</v>
+      </c>
+      <c r="M2">
+        <f>ABS(Table2[[#This Row],[Marin]]-L2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -596,11 +693,37 @@
       <c r="D3">
         <v>86</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>76</v>
+      </c>
+      <c r="I3">
+        <v>75</v>
+      </c>
+      <c r="J3">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H3)</f>
+        <v>26</v>
+      </c>
+      <c r="K3">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I3)</f>
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L17" si="0">ABS(H3-I3)</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>ABS(Table2[[#This Row],[Marin]]-L3)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -613,11 +736,37 @@
       <c r="D4">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>89</v>
+      </c>
+      <c r="I4">
+        <v>68</v>
+      </c>
+      <c r="J4">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H4)</f>
+        <v>17</v>
+      </c>
+      <c r="K4">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I4)</f>
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="M4">
+        <f>ABS(Table2[[#This Row],[Marin]]-L4)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -630,11 +779,37 @@
       <c r="D5">
         <v>64</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>77</v>
+      </c>
+      <c r="I5">
+        <v>74</v>
+      </c>
+      <c r="J5">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H5)</f>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I5)</f>
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <f>ABS(Table2[[#This Row],[Marin]]-L5)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -647,11 +822,37 @@
       <c r="D6">
         <v>65</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>77</v>
+      </c>
+      <c r="I6">
+        <v>71</v>
+      </c>
+      <c r="J6">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H6)</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I6)</f>
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <f>ABS(Table2[[#This Row],[Marin]]-L6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -664,11 +865,37 @@
       <c r="D7">
         <v>72</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>74</v>
+      </c>
+      <c r="I7">
+        <v>70</v>
+      </c>
+      <c r="J7">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H7)</f>
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I7)</f>
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <f>ABS(Table2[[#This Row],[Marin]]-L7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -681,11 +908,37 @@
       <c r="D8">
         <v>59</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>88</v>
+      </c>
+      <c r="I8">
+        <v>67</v>
+      </c>
+      <c r="J8">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H8)</f>
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I8)</f>
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="M8">
+        <f>ABS(Table2[[#This Row],[Marin]]-L8)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -698,11 +951,37 @@
       <c r="D9">
         <v>67</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>103</v>
+      </c>
+      <c r="I9">
+        <v>64</v>
+      </c>
+      <c r="J9">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H9)</f>
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I9)</f>
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="M9">
+        <f>ABS(Table2[[#This Row],[Marin]]-L9)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -715,11 +994,37 @@
       <c r="D10">
         <v>74</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>75</v>
+      </c>
+      <c r="I10">
+        <v>70</v>
+      </c>
+      <c r="J10">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H10)</f>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I10)</f>
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <f>ABS(Table2[[#This Row],[Marin]]-L10)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -732,11 +1037,37 @@
       <c r="D11">
         <v>79</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>70</v>
+      </c>
+      <c r="J11">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H11)</f>
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I11)</f>
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <f>ABS(Table2[[#This Row],[Marin]]-L11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -749,11 +1080,37 @@
       <c r="D12">
         <v>64</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>89</v>
+      </c>
+      <c r="I12">
+        <v>67</v>
+      </c>
+      <c r="J12">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H12)</f>
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I12)</f>
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="M12">
+        <f>ABS(Table2[[#This Row],[Marin]]-L12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -766,11 +1123,37 @@
       <c r="D13">
         <v>58</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>73</v>
+      </c>
+      <c r="I13">
+        <v>67</v>
+      </c>
+      <c r="J13">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H13)</f>
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I13)</f>
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M13">
+        <f>ABS(Table2[[#This Row],[Marin]]-L13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -783,11 +1166,37 @@
       <c r="D14">
         <v>80</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>87</v>
+      </c>
+      <c r="I14">
+        <v>72</v>
+      </c>
+      <c r="J14">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H14)</f>
+        <v>28</v>
+      </c>
+      <c r="K14">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I14)</f>
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <f>ABS(Table2[[#This Row],[Marin]]-L14)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -800,11 +1209,37 @@
       <c r="D15">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>90</v>
+      </c>
+      <c r="I15">
+        <v>64</v>
+      </c>
+      <c r="J15">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H15)</f>
+        <v>18</v>
+      </c>
+      <c r="K15">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I15)</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="M15">
+        <f>ABS(Table2[[#This Row],[Marin]]-L15)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -817,11 +1252,37 @@
       <c r="D16">
         <v>69</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>75</v>
+      </c>
+      <c r="I16">
+        <v>74</v>
+      </c>
+      <c r="J16">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H16)</f>
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I16)</f>
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f>ABS(Table2[[#This Row],[Marin]]-L16)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -834,14 +1295,381 @@
       <c r="D17">
         <v>72</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
         <v>23</v>
+      </c>
+      <c r="H17">
+        <v>75</v>
+      </c>
+      <c r="I17">
+        <v>72</v>
+      </c>
+      <c r="J17">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H17)</f>
+        <v>7</v>
+      </c>
+      <c r="K17">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I17)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <f>ABS(Table2[[#This Row],[Marin]]-L17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>76</v>
+      </c>
+      <c r="I18">
+        <v>71</v>
+      </c>
+      <c r="J18">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H18)</f>
+        <v>76</v>
+      </c>
+      <c r="K18">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I18)</f>
+        <v>71</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L27" si="1">ABS(H18-I18)</f>
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <f>ABS(Table2[[#This Row],[Marin]]-L18)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>74</v>
+      </c>
+      <c r="I19">
+        <v>70</v>
+      </c>
+      <c r="J19">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H19)</f>
+        <v>74</v>
+      </c>
+      <c r="K19">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I19)</f>
+        <v>70</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <f>ABS(Table2[[#This Row],[Marin]]-L19)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>77</v>
+      </c>
+      <c r="I20">
+        <v>73</v>
+      </c>
+      <c r="J20">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H20)</f>
+        <v>77</v>
+      </c>
+      <c r="K20">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I20)</f>
+        <v>73</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f>ABS(Table2[[#This Row],[Marin]]-L20)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>75</v>
+      </c>
+      <c r="I21">
+        <v>71</v>
+      </c>
+      <c r="J21">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H21)</f>
+        <v>75</v>
+      </c>
+      <c r="K21">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I21)</f>
+        <v>71</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <f>ABS(Table2[[#This Row],[Marin]]-L21)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>76</v>
+      </c>
+      <c r="I22">
+        <v>73</v>
+      </c>
+      <c r="J22">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H22)</f>
+        <v>76</v>
+      </c>
+      <c r="K22">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I22)</f>
+        <v>73</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <f>ABS(Table2[[#This Row],[Marin]]-L22)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>76</v>
+      </c>
+      <c r="I23">
+        <v>73</v>
+      </c>
+      <c r="J23">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H23)</f>
+        <v>76</v>
+      </c>
+      <c r="K23">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I23)</f>
+        <v>73</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <f>ABS(Table2[[#This Row],[Marin]]-L23)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>74</v>
+      </c>
+      <c r="I24">
+        <v>81</v>
+      </c>
+      <c r="J24">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H24)</f>
+        <v>74</v>
+      </c>
+      <c r="K24">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I24)</f>
+        <v>81</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M24">
+        <f>ABS(Table2[[#This Row],[Marin]]-L24)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>71</v>
+      </c>
+      <c r="I25">
+        <v>70</v>
+      </c>
+      <c r="J25">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H25)</f>
+        <v>71</v>
+      </c>
+      <c r="K25">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I25)</f>
+        <v>70</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f>ABS(Table2[[#This Row],[Marin]]-L25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>82</v>
+      </c>
+      <c r="I26">
+        <v>74</v>
+      </c>
+      <c r="J26">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H26)</f>
+        <v>82</v>
+      </c>
+      <c r="K26">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I26)</f>
+        <v>74</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <f>ABS(Table2[[#This Row],[Marin]]-L26)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <f>ABS(Table2[[#This Row],[Home Points]]-Table2[[#This Row],[Away Points]])</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>73</v>
+      </c>
+      <c r="I27">
+        <v>70</v>
+      </c>
+      <c r="J27">
+        <f>ABS(Table2[[#This Row],[Home Points]]-H27)</f>
+        <v>73</v>
+      </c>
+      <c r="K27">
+        <f>ABS(Table2[[#This Row],[Away Points]]-I27)</f>
+        <v>70</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <f>ABS(Table2[[#This Row],[Marin]]-L27)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>